<commit_message>
Particles.js en kleur feature
</commit_message>
<xml_diff>
--- a/files/Test1234/converted/Bestand2.xlsx
+++ b/files/Test1234/converted/Bestand2.xlsx
@@ -399,7 +399,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bestand 1 column 4</t>
+          <t>dwadwaBestand 1 column 4</t>
         </is>
       </c>
     </row>
@@ -433,7 +433,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bestand 1 column 6</t>
+          <t>dadaBestand 1 column 6</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bestand 1 column 2</t>
+          <t>adaBestand 1 column 2</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Bestand 1 column 8</t>
+          <t>dadaBestand 1 column 8</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bestand 1 column 11</t>
+          <t>dadaBestand 1 column 11</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bestand 1 column 10</t>
+          <t>dadaBestand 1 column 10</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bestand 1 column 9</t>
+          <t>adaBestand 1 column 9</t>
         </is>
       </c>
     </row>

</xml_diff>